<commit_message>
Weekly plan turn in 30 March 2018
</commit_message>
<xml_diff>
--- a/GUMen'sBasketballYahtzeeGroupProjectPlan.xlsx
+++ b/GUMen'sBasketballYahtzeeGroupProjectPlan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EugeneKrug/Documents/School/Spring_2018/CPSC_224_Zhang/Group_Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EugeneKrug/Documents/GitHub/CPSC224GroupProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B93338-3620-FB47-9848-BA92B839B4F1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F155E1-4B76-DB4A-90F6-F8F9FE98FEE6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38320" windowHeight="19840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38320" windowHeight="19840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="25March" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
   <si>
     <t>Task</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>After group review and approval, turn in Project Plan to Blackboard (weekly)</t>
+  </si>
+  <si>
+    <t>ASAP</t>
   </si>
 </sst>
 </file>
@@ -151,15 +154,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -443,8 +453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView zoomScale="146" zoomScaleNormal="146" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" zoomScale="189" zoomScaleNormal="189" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -453,228 +463,266 @@
     <col min="2" max="7" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" ht="31.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="31.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D2" s="4">
+        <v>43189</v>
+      </c>
+      <c r="E2" s="5">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4">
+        <v>43186</v>
+      </c>
+      <c r="E3" s="5">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4">
+        <v>43184</v>
+      </c>
+      <c r="G3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4">
+        <v>43186</v>
+      </c>
+      <c r="E4" s="5">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4">
+        <v>43184</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2">
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4">
+        <v>43186</v>
+      </c>
+      <c r="E5" s="5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4">
+        <v>43186</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="D6" s="4">
+        <v>43187</v>
+      </c>
+      <c r="E6" s="5">
+        <v>1</v>
+      </c>
+      <c r="F6" s="4">
+        <v>43186</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D7" s="4">
         <v>43189</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="E7" s="5">
+        <v>1</v>
+      </c>
+      <c r="F7" s="4">
+        <v>43189</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2">
-        <v>43186</v>
-      </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2">
-        <v>43186</v>
-      </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2">
-        <v>43186</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0.15</v>
-      </c>
-      <c r="D6" s="2">
-        <v>43187</v>
-      </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="D7" s="2">
+      <c r="C8" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="D8" s="4">
         <v>43189</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0.15</v>
-      </c>
-      <c r="D8" s="2">
+      <c r="E8" s="5">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4">
         <v>43189</v>
       </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="G8" s="3">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -688,10 +736,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB69CEBE-E69E-C34D-85ED-8CEEE09558EB}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -700,212 +748,229 @@
     <col min="2" max="7" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" ht="31.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="31.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:7" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C3" s="3">
         <v>2</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D3" s="4">
         <v>43196</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1">
-        <v>0.15</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="C4" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="D4" s="4">
         <v>43196</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C5" s="3">
         <v>4</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D5" s="4">
         <v>43196</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1">
-        <v>0.15</v>
-      </c>
-      <c r="D5" s="2">
+      <c r="C6" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="D6" s="4">
         <v>43196</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="1">
-        <v>0.15</v>
-      </c>
-      <c r="D6" s="2">
+      <c r="C7" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="D7" s="4">
         <v>43196</v>
       </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -913,12 +978,30 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Doc_x0020_Type xmlns="9b0d329a-e114-4ba8-bee9-62c1c786fd9a">
+      <Value>Group Project</Value>
+    </Doc_x0020_Type>
+    <SharedWithUsers xmlns="013b2221-5078-4f34-9921-a0ecb049492d">
+      <UserInfo>
+        <DisplayName>Greenside, Trevor Michael</DisplayName>
+        <AccountId>146</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Kopczynski, Scott Patrick</DisplayName>
+        <AccountId>609</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Hartwell, Harvey C</DisplayName>
+        <AccountId>606</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1103,36 +1186,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Doc_x0020_Type xmlns="9b0d329a-e114-4ba8-bee9-62c1c786fd9a">
-      <Value>Group Project</Value>
-    </Doc_x0020_Type>
-    <SharedWithUsers xmlns="013b2221-5078-4f34-9921-a0ecb049492d">
-      <UserInfo>
-        <DisplayName>Greenside, Trevor Michael</DisplayName>
-        <AccountId>146</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Kopczynski, Scott Patrick</DisplayName>
-        <AccountId>609</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Hartwell, Harvey C</DisplayName>
-        <AccountId>606</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{977C615D-C0CF-4E54-82E4-40DCE513F318}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B616F827-B535-4D73-8E2B-1E3703C34EC5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9b0d329a-e114-4ba8-bee9-62c1c786fd9a"/>
+    <ds:schemaRef ds:uri="013b2221-5078-4f34-9921-a0ecb049492d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1157,12 +1225,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B616F827-B535-4D73-8E2B-1E3703C34EC5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{977C615D-C0CF-4E54-82E4-40DCE513F318}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9b0d329a-e114-4ba8-bee9-62c1c786fd9a"/>
-    <ds:schemaRef ds:uri="013b2221-5078-4f34-9921-a0ecb049492d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Weekly plan turn in on 30 March 2018
</commit_message>
<xml_diff>
--- a/GUMen'sBasketballYahtzeeGroupProjectPlan.xlsx
+++ b/GUMen'sBasketballYahtzeeGroupProjectPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EugeneKrug/Documents/GitHub/CPSC224GroupProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F155E1-4B76-DB4A-90F6-F8F9FE98FEE6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC26A399-2B52-3E46-824E-A746E6D1D5A6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38320" windowHeight="19840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -453,8 +453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="189" zoomScaleNormal="189" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="189" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -728,8 +728,8 @@
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;LCPSC 224
-As of:  latestUpdateDate&amp;CProject Plan&amp;RProject: projectName</oddHeader>
+    <oddHeader xml:space="preserve">&amp;LGonzaga Men's Basketball Yahtzee&amp;C&amp;"System Font,Regular"&amp;10&amp;K000000Group Project Plan&amp;R&amp;"System Font,Regular"&amp;10&amp;K000000Benjamin Bladow, Brandon Niblock, Eugene Krug
+</oddHeader>
   </headerFooter>
 </worksheet>
 </file>
@@ -978,33 +978,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Doc_x0020_Type xmlns="9b0d329a-e114-4ba8-bee9-62c1c786fd9a">
-      <Value>Group Project</Value>
-    </Doc_x0020_Type>
-    <SharedWithUsers xmlns="013b2221-5078-4f34-9921-a0ecb049492d">
-      <UserInfo>
-        <DisplayName>Greenside, Trevor Michael</DisplayName>
-        <AccountId>146</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Kopczynski, Scott Patrick</DisplayName>
-        <AccountId>609</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Hartwell, Harvey C</DisplayName>
-        <AccountId>606</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AC2685C84B160940930467983553E2DA" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="64476ae877ed79da2175079bb3e4829a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9b0d329a-e114-4ba8-bee9-62c1c786fd9a" xmlns:ns3="013b2221-5078-4f34-9921-a0ecb049492d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="564df3335efcf36b4d09ae51e046af81" ns2:_="" ns3:_="">
     <xsd:import namespace="9b0d329a-e114-4ba8-bee9-62c1c786fd9a"/>
@@ -1185,6 +1158,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Doc_x0020_Type xmlns="9b0d329a-e114-4ba8-bee9-62c1c786fd9a">
+      <Value>Group Project</Value>
+    </Doc_x0020_Type>
+    <SharedWithUsers xmlns="013b2221-5078-4f34-9921-a0ecb049492d">
+      <UserInfo>
+        <DisplayName>Greenside, Trevor Michael</DisplayName>
+        <AccountId>146</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Kopczynski, Scott Patrick</DisplayName>
+        <AccountId>609</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Hartwell, Harvey C</DisplayName>
+        <AccountId>606</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1195,17 +1195,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B616F827-B535-4D73-8E2B-1E3703C34EC5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9b0d329a-e114-4ba8-bee9-62c1c786fd9a"/>
-    <ds:schemaRef ds:uri="013b2221-5078-4f34-9921-a0ecb049492d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{309F765C-3428-4D4C-A6F6-5C1534E87CBC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1224,6 +1213,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B616F827-B535-4D73-8E2B-1E3703C34EC5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9b0d329a-e114-4ba8-bee9-62c1c786fd9a"/>
+    <ds:schemaRef ds:uri="013b2221-5078-4f34-9921-a0ecb049492d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{977C615D-C0CF-4E54-82E4-40DCE513F318}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Weekly Plan Update 6 April 2018
</commit_message>
<xml_diff>
--- a/GUMen'sBasketballYahtzeeGroupProjectPlan.xlsx
+++ b/GUMen'sBasketballYahtzeeGroupProjectPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EugeneKrug/Documents/GitHub/CPSC224_02_Group1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2CD8456-5390-BE47-9003-7BE824A999F3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5095BE8-55FD-DB4B-8302-AEB68CEC2312}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38220" windowHeight="20080" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="25 March 2018" sheetId="1" r:id="rId1"/>
@@ -777,7 +777,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="132" zoomScaleNormal="148" zoomScalePageLayoutView="132" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -845,9 +845,15 @@
       <c r="D3" s="4">
         <v>43196</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="E3" s="5">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4">
+        <v>43196</v>
+      </c>
+      <c r="G3" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
@@ -862,9 +868,15 @@
       <c r="D4" s="4">
         <v>43196</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="E4" s="5">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4">
+        <v>43196</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
@@ -932,7 +944,7 @@
         <v>43195</v>
       </c>
       <c r="G7" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -948,9 +960,15 @@
       <c r="D8" s="4">
         <v>43196</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
+      <c r="E8" s="5">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4">
+        <v>43196</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
@@ -1066,7 +1084,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScale="150" zoomScaleNormal="210" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1396,6 +1414,42 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Doc_x0020_Type xmlns="9b0d329a-e114-4ba8-bee9-62c1c786fd9a">
+      <Value>Group Project</Value>
+    </Doc_x0020_Type>
+    <SharedWithUsers xmlns="013b2221-5078-4f34-9921-a0ecb049492d">
+      <UserInfo>
+        <DisplayName>Greenside, Trevor Michael</DisplayName>
+        <AccountId>146</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Kopczynski, Scott Patrick</DisplayName>
+        <AccountId>609</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Hartwell, Harvey C</DisplayName>
+        <AccountId>606</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AC2685C84B160940930467983553E2DA" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="64476ae877ed79da2175079bb3e4829a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9b0d329a-e114-4ba8-bee9-62c1c786fd9a" xmlns:ns3="013b2221-5078-4f34-9921-a0ecb049492d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="564df3335efcf36b4d09ae51e046af81" ns2:_="" ns3:_="">
     <xsd:import namespace="9b0d329a-e114-4ba8-bee9-62c1c786fd9a"/>
@@ -1576,43 +1630,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Doc_x0020_Type xmlns="9b0d329a-e114-4ba8-bee9-62c1c786fd9a">
-      <Value>Group Project</Value>
-    </Doc_x0020_Type>
-    <SharedWithUsers xmlns="013b2221-5078-4f34-9921-a0ecb049492d">
-      <UserInfo>
-        <DisplayName>Greenside, Trevor Michael</DisplayName>
-        <AccountId>146</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Kopczynski, Scott Patrick</DisplayName>
-        <AccountId>609</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Hartwell, Harvey C</DisplayName>
-        <AccountId>606</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{977C615D-C0CF-4E54-82E4-40DCE513F318}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B616F827-B535-4D73-8E2B-1E3703C34EC5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9b0d329a-e114-4ba8-bee9-62c1c786fd9a"/>
+    <ds:schemaRef ds:uri="013b2221-5078-4f34-9921-a0ecb049492d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{309F765C-3428-4D4C-A6F6-5C1534E87CBC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1629,23 +1666,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B616F827-B535-4D73-8E2B-1E3703C34EC5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9b0d329a-e114-4ba8-bee9-62c1c786fd9a"/>
-    <ds:schemaRef ds:uri="013b2221-5078-4f34-9921-a0ecb049492d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{977C615D-C0CF-4E54-82E4-40DCE513F318}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Project plan updated 20 April 2018
</commit_message>
<xml_diff>
--- a/GUMen'sBasketballYahtzeeGroupProjectPlan.xlsx
+++ b/GUMen'sBasketballYahtzeeGroupProjectPlan.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EugeneKrug/Documents/GitHub/CPSC224_02_Group1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24847903-8D04-124D-BF28-DDD971604547}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F81891DE-5714-7440-AFAC-236C69C6AD73}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38220" windowHeight="19880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14760" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="25 March 2018" sheetId="1" r:id="rId1"/>
     <sheet name="1 April 2018" sheetId="2" r:id="rId2"/>
     <sheet name="8 April 2018" sheetId="4" r:id="rId3"/>
     <sheet name="15 April 2018" sheetId="5" r:id="rId4"/>
+    <sheet name="22 April 2018" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="44">
   <si>
     <t>Task</t>
   </si>
@@ -144,13 +145,22 @@
     <t>Test code in non-GUI environment</t>
   </si>
   <si>
-    <t>Work on 1/3 of the GUI: Scoreboard</t>
-  </si>
-  <si>
-    <t>Work on 1/3 of the GUI: Rolls</t>
-  </si>
-  <si>
-    <t>Work on 1/3 of the GUI: Main Menu, Leaderboard, Instructions</t>
+    <t>GUI: Main Menu, Leaderboard, Instructions, Beginning Game</t>
+  </si>
+  <si>
+    <t>Finish GUI Implementation</t>
+  </si>
+  <si>
+    <t>Final Game Testing</t>
+  </si>
+  <si>
+    <t>Begin testing with Junit</t>
+  </si>
+  <si>
+    <t>Begin presentation</t>
+  </si>
+  <si>
+    <t>Begin final report</t>
   </si>
 </sst>
 </file>
@@ -1099,7 +1109,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D56F2DE1-106B-9644-B9E6-E5F6AF9A6452}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="150" zoomScaleNormal="210" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView view="pageLayout" zoomScale="150" zoomScaleNormal="210" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -1572,10 +1582,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5119451F-DC30-0241-9B4C-92E3624495E3}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1622,13 +1632,19 @@
       <c r="D2" s="4">
         <v>43209</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="3"/>
+      <c r="E2" s="5">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4">
+        <v>43209</v>
+      </c>
+      <c r="G2" s="3">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>12</v>
@@ -1639,13 +1655,19 @@
       <c r="D3" s="4">
         <v>43209</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="3"/>
+      <c r="E3" s="5">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4">
+        <v>43209</v>
+      </c>
+      <c r="G3" s="3">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>10</v>
@@ -1656,35 +1678,61 @@
       <c r="D4" s="4">
         <v>43209</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="3"/>
+      <c r="E4" s="5">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4">
+        <v>43209</v>
+      </c>
+      <c r="G4" s="3">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4">
+        <v>43209</v>
+      </c>
+      <c r="E5" s="5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4">
+        <v>43209</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C6" s="3">
         <v>0.25</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D6" s="4">
         <v>43210</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="3"/>
+      <c r="E6" s="5">
+        <v>1</v>
+      </c>
+      <c r="F6" s="4">
+        <v>43210</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
@@ -1762,9 +1810,9 @@
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="4"/>
       <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -1847,6 +1895,354 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <headerFooter>
+    <oddHeader>&amp;LGonzaga Men's Basketball Yahtzee
+Group Project Plan&amp;RBenjamin Bladow, Brandon Niblock, Eugene Krug</oddHeader>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0325AA8A-3BD8-9A4C-A76E-CD25D090145C}">
+  <dimension ref="A1:G27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="50.1640625" customWidth="1"/>
+    <col min="2" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="15.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="31.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3">
+        <v>4</v>
+      </c>
+      <c r="D2" s="4">
+        <v>43216</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3">
+        <v>4</v>
+      </c>
+      <c r="D3" s="4">
+        <v>43216</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3">
+        <v>4</v>
+      </c>
+      <c r="D4" s="4">
+        <v>43216</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3">
+        <v>4</v>
+      </c>
+      <c r="D5" s="4">
+        <v>43216</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2</v>
+      </c>
+      <c r="D6" s="4">
+        <v>43216</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="3">
+        <v>2</v>
+      </c>
+      <c r="D7" s="4">
+        <v>43216</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="D8" s="4">
+        <v>43217</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1859,6 +2255,33 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Doc_x0020_Type xmlns="9b0d329a-e114-4ba8-bee9-62c1c786fd9a">
+      <Value>Group Project</Value>
+    </Doc_x0020_Type>
+    <SharedWithUsers xmlns="013b2221-5078-4f34-9921-a0ecb049492d">
+      <UserInfo>
+        <DisplayName>Greenside, Trevor Michael</DisplayName>
+        <AccountId>146</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Kopczynski, Scott Patrick</DisplayName>
+        <AccountId>609</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Hartwell, Harvey C</DisplayName>
+        <AccountId>606</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AC2685C84B160940930467983553E2DA" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="64476ae877ed79da2175079bb3e4829a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9b0d329a-e114-4ba8-bee9-62c1c786fd9a" xmlns:ns3="013b2221-5078-4f34-9921-a0ecb049492d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="564df3335efcf36b4d09ae51e046af81" ns2:_="" ns3:_="">
     <xsd:import namespace="9b0d329a-e114-4ba8-bee9-62c1c786fd9a"/>
@@ -2039,33 +2462,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Doc_x0020_Type xmlns="9b0d329a-e114-4ba8-bee9-62c1c786fd9a">
-      <Value>Group Project</Value>
-    </Doc_x0020_Type>
-    <SharedWithUsers xmlns="013b2221-5078-4f34-9921-a0ecb049492d">
-      <UserInfo>
-        <DisplayName>Greenside, Trevor Michael</DisplayName>
-        <AccountId>146</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Kopczynski, Scott Patrick</DisplayName>
-        <AccountId>609</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Hartwell, Harvey C</DisplayName>
-        <AccountId>606</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2076,6 +2472,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B616F827-B535-4D73-8E2B-1E3703C34EC5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9b0d329a-e114-4ba8-bee9-62c1c786fd9a"/>
+    <ds:schemaRef ds:uri="013b2221-5078-4f34-9921-a0ecb049492d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{309F765C-3428-4D4C-A6F6-5C1534E87CBC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2094,17 +2501,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B616F827-B535-4D73-8E2B-1E3703C34EC5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9b0d329a-e114-4ba8-bee9-62c1c786fd9a"/>
-    <ds:schemaRef ds:uri="013b2221-5078-4f34-9921-a0ecb049492d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{977C615D-C0CF-4E54-82E4-40DCE513F318}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
code & project plan updated
</commit_message>
<xml_diff>
--- a/GUMen'sBasketballYahtzeeGroupProjectPlan.xlsx
+++ b/GUMen'sBasketballYahtzeeGroupProjectPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EugeneKrug/Documents/GitHub/CPSC224_02_Group1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F81891DE-5714-7440-AFAC-236C69C6AD73}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F10828AA-032C-DE4F-9A44-04866C468242}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14760" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19820" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="25 March 2018" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="8 April 2018" sheetId="4" r:id="rId3"/>
     <sheet name="15 April 2018" sheetId="5" r:id="rId4"/>
     <sheet name="22 April 2018" sheetId="6" r:id="rId5"/>
+    <sheet name="29 April 2018" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="55">
   <si>
     <t>Task</t>
   </si>
@@ -157,10 +158,43 @@
     <t>Begin testing with Junit</t>
   </si>
   <si>
-    <t>Begin presentation</t>
-  </si>
-  <si>
     <t>Begin final report</t>
+  </si>
+  <si>
+    <t>100%%</t>
+  </si>
+  <si>
+    <t>Turn In Deadline: Complete code on ADA</t>
+  </si>
+  <si>
+    <t>Turn In Deadline: Powerpoint</t>
+  </si>
+  <si>
+    <t>Turn In Deadline: Final Report</t>
+  </si>
+  <si>
+    <t>Clean up code to prepare for turn in</t>
+  </si>
+  <si>
+    <t>4/29/18*</t>
+  </si>
+  <si>
+    <t>JUnit Testing</t>
+  </si>
+  <si>
+    <t>Turn In Deadline: JUnit Testing (Code/Screenshots) &amp; GItHub (screenshots)</t>
+  </si>
+  <si>
+    <t>Create Powerpoint</t>
+  </si>
+  <si>
+    <t>UML Sequence Diagram</t>
+  </si>
+  <si>
+    <t>Final Report (revise existing components as necessary)</t>
+  </si>
+  <si>
+    <t>*We intend to have everything done by the end of the day on Sunday, 29 April.</t>
   </si>
 </sst>
 </file>
@@ -217,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -232,6 +266,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1917,10 +1960,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0325AA8A-3BD8-9A4C-A76E-CD25D090145C}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1967,9 +2010,15 @@
       <c r="D2" s="4">
         <v>43216</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="3"/>
+      <c r="E2" s="5">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4">
+        <v>43216</v>
+      </c>
+      <c r="G2" s="3">
+        <v>12</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -1984,9 +2033,15 @@
       <c r="D3" s="4">
         <v>43216</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="3"/>
+      <c r="E3" s="5">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4">
+        <v>43216</v>
+      </c>
+      <c r="G3" s="3">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
@@ -2001,9 +2056,15 @@
       <c r="D4" s="4">
         <v>43216</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="3"/>
+      <c r="E4" s="5">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4">
+        <v>43216</v>
+      </c>
+      <c r="G4" s="3">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
@@ -2018,16 +2079,22 @@
       <c r="D5" s="4">
         <v>43216</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="3"/>
+      <c r="E5" s="5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4">
+        <v>43216</v>
+      </c>
+      <c r="G5" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C6" s="3">
         <v>2</v>
@@ -2035,16 +2102,22 @@
       <c r="D6" s="4">
         <v>43216</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="3"/>
+      <c r="E6" s="5">
+        <v>1</v>
+      </c>
+      <c r="F6" s="4">
+        <v>43216</v>
+      </c>
+      <c r="G6" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C7" s="3">
         <v>2</v>
@@ -2052,35 +2125,61 @@
       <c r="D7" s="4">
         <v>43216</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="3"/>
+      <c r="E7" s="5">
+        <v>1</v>
+      </c>
+      <c r="F7" s="4">
+        <v>43216</v>
+      </c>
+      <c r="G7" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="3">
+        <v>2</v>
+      </c>
+      <c r="D8" s="4">
+        <v>43216</v>
+      </c>
+      <c r="E8" s="5">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4">
+        <v>43217</v>
+      </c>
+      <c r="G8" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="3">
         <v>0.25</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D9" s="4">
         <v>43217</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="3"/>
+      <c r="E9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="4">
+        <v>43217</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
@@ -2158,9 +2257,9 @@
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="4"/>
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -2243,6 +2342,273 @@
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <headerFooter>
+    <oddHeader>&amp;LGonzaga Men's Basketball Yahtzee
+Group Project Plan&amp;RBenjamin Bladow, Brandon Niblock, Eugene Krug</oddHeader>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24A4F457-0DF1-0E47-B48A-F8E960528D7A}">
+  <dimension ref="A1:G15"/>
+  <sheetViews>
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="59.83203125" customWidth="1"/>
+    <col min="2" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="15.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="31.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="D5" s="4">
+        <v>43224</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3">
+        <v>3</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="D7" s="4">
+        <v>43224</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="3">
+        <v>2</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="3">
+        <v>2</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="D10" s="4">
+        <v>43223</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="3">
+        <v>2</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="3">
+        <v>4</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="D13" s="4">
+        <v>43227</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
+        <v>54</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2255,30 +2621,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Doc_x0020_Type xmlns="9b0d329a-e114-4ba8-bee9-62c1c786fd9a">
-      <Value>Group Project</Value>
-    </Doc_x0020_Type>
-    <SharedWithUsers xmlns="013b2221-5078-4f34-9921-a0ecb049492d">
-      <UserInfo>
-        <DisplayName>Greenside, Trevor Michael</DisplayName>
-        <AccountId>146</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Kopczynski, Scott Patrick</DisplayName>
-        <AccountId>609</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Hartwell, Harvey C</DisplayName>
-        <AccountId>606</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2463,21 +2811,36 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Doc_x0020_Type xmlns="9b0d329a-e114-4ba8-bee9-62c1c786fd9a">
+      <Value>Group Project</Value>
+    </Doc_x0020_Type>
+    <SharedWithUsers xmlns="013b2221-5078-4f34-9921-a0ecb049492d">
+      <UserInfo>
+        <DisplayName>Greenside, Trevor Michael</DisplayName>
+        <AccountId>146</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Kopczynski, Scott Patrick</DisplayName>
+        <AccountId>609</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Hartwell, Harvey C</DisplayName>
+        <AccountId>606</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B616F827-B535-4D73-8E2B-1E3703C34EC5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{977C615D-C0CF-4E54-82E4-40DCE513F318}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9b0d329a-e114-4ba8-bee9-62c1c786fd9a"/>
-    <ds:schemaRef ds:uri="013b2221-5078-4f34-9921-a0ecb049492d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2502,9 +2865,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{977C615D-C0CF-4E54-82E4-40DCE513F318}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B616F827-B535-4D73-8E2B-1E3703C34EC5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9b0d329a-e114-4ba8-bee9-62c1c786fd9a"/>
+    <ds:schemaRef ds:uri="013b2221-5078-4f34-9921-a0ecb049492d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>